<commit_message>
Updated Q7 excel file
added constraints
</commit_message>
<xml_diff>
--- a/IE407-Q7.xlsx
+++ b/IE407-Q7.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AlpErenYılmaz\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eheng\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{547F48EC-72F2-40D2-A607-A100032096F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D45286B-FCDB-48EE-BB0B-DF7F4F42C341}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-118" yWindow="-118" windowWidth="25370" windowHeight="14374" activeTab="1" xr2:uid="{29C75357-6D86-4F34-87D3-5ABA805A4EC9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{29C75357-6D86-4F34-87D3-5ABA805A4EC9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1 Sensitivity" sheetId="2" r:id="rId1"/>
@@ -28,6 +28,7 @@
     <definedName name="solver_itr" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_lhs1" localSheetId="1" hidden="1">Sayfa1!$C$63:$C$87</definedName>
     <definedName name="solver_lhs10" localSheetId="1" hidden="1">Sayfa1!$BD$6:$BH$30</definedName>
+    <definedName name="solver_lhs11" localSheetId="1" hidden="1">Sayfa1!$W$72:$W$76</definedName>
     <definedName name="solver_lhs2" localSheetId="1" hidden="1">Sayfa1!$H$63:$H$87</definedName>
     <definedName name="solver_lhs3" localSheetId="1" hidden="1">Sayfa1!$M$63:$M$87</definedName>
     <definedName name="solver_lhs4" localSheetId="1" hidden="1">Sayfa1!$R$63:$R$67</definedName>
@@ -37,11 +38,12 @@
     <definedName name="solver_lhs8" localSheetId="1" hidden="1">Sayfa1!$AP$6:$AT$30</definedName>
     <definedName name="solver_lhs9" localSheetId="1" hidden="1">Sayfa1!$AW$6:$BA$30</definedName>
     <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_num" localSheetId="1" hidden="1">10</definedName>
+    <definedName name="solver_num" localSheetId="1" hidden="1">11</definedName>
     <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_opt" localSheetId="1" hidden="1">Sayfa1!$B$55</definedName>
     <definedName name="solver_rel1" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel10" localSheetId="1" hidden="1">5</definedName>
+    <definedName name="solver_rel11" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rel2" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_rel3" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel4" localSheetId="1" hidden="1">1</definedName>
@@ -52,6 +54,7 @@
     <definedName name="solver_rel9" localSheetId="1" hidden="1">5</definedName>
     <definedName name="solver_rhs1" localSheetId="1" hidden="1">Sayfa1!$E$63:$E$87</definedName>
     <definedName name="solver_rhs10" localSheetId="1" hidden="1">binary</definedName>
+    <definedName name="solver_rhs11" localSheetId="1" hidden="1">Sayfa1!$Y$72:$Y$76</definedName>
     <definedName name="solver_rhs2" localSheetId="1" hidden="1">Sayfa1!$J$63:$J$87</definedName>
     <definedName name="solver_rhs3" localSheetId="1" hidden="1">Sayfa1!$O$63:$O$87</definedName>
     <definedName name="solver_rhs4" localSheetId="1" hidden="1">Sayfa1!$T$63:$T$67</definedName>
@@ -109,7 +112,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1862" uniqueCount="1166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1868" uniqueCount="1167">
   <si>
     <t>INDICES</t>
   </si>
@@ -3607,6 +3610,9 @@
   </si>
   <si>
     <t>used for objective function</t>
+  </si>
+  <si>
+    <t>7-New Constrain: Products 3 and 8 must be in the same shelf if assorted</t>
   </si>
 </sst>
 </file>
@@ -4104,10 +4110,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="OpenSolver1">
+        <xdr:cNvPr id="78" name="OpenSolver1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BECCAB99-9C4D-424C-9948-849D3B918458}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1ABC0328-A141-4652-A514-70507B79AE26}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4192,10 +4198,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="OpenSolver2">
+        <xdr:cNvPr id="79" name="OpenSolver2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{960B0994-F036-4707-8AFF-499FBFC05B33}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A342B5E4-F544-417B-91BA-803256B6126B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4280,10 +4286,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="OpenSolver3">
+        <xdr:cNvPr id="80" name="OpenSolver3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F396E916-0186-44C3-88AF-33B27241D5B5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{19D921BF-082B-47C2-AB76-CFFE18562C11}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4368,10 +4374,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="OpenSolver4">
+        <xdr:cNvPr id="81" name="OpenSolver4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{26048256-20E1-4C59-8760-BEC3883CF779}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C2CBDDFC-AFE5-4E65-955B-D33FE6AF90A1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4456,10 +4462,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="OpenSolver5">
+        <xdr:cNvPr id="82" name="OpenSolver5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F04332CE-B091-4038-80A5-73AC1876CA5E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B4FCC519-DF5B-4D59-89D1-E9707772DBE7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4538,10 +4544,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="OpenSolver6">
+        <xdr:cNvPr id="83" name="OpenSolver6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{68D2BAD5-632A-4BDE-8D37-01703A26518A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1F7A098-5BF3-4AFA-B250-DB8AEE8C92B0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4631,10 +4637,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="OpenSolver7">
+        <xdr:cNvPr id="84" name="OpenSolver7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A20E9D7B-8D59-448C-AED6-241E07420EDF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C4B7D13-4FEA-4F75-8B5E-FFFDC2C9EB96}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4713,10 +4719,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="OpenSolver8">
+        <xdr:cNvPr id="85" name="OpenSolver8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A2326FCA-2571-4C00-8935-EAF1BAF5EC09}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{213B9961-A24B-4325-8794-85AE6E511D86}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4798,16 +4804,16 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="10" name="OpenSolver9">
+        <xdr:cNvPr id="86" name="OpenSolver9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE3CB8E7-5CD6-4ADC-B56F-7C08FF9D318E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{36E13004-7DB2-49E4-B4F7-C41D0736D046}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="8" idx="3"/>
-          <a:endCxn id="9" idx="1"/>
+          <a:stCxn id="84" idx="3"/>
+          <a:endCxn id="85" idx="1"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -4859,10 +4865,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="OpenSolver10">
+        <xdr:cNvPr id="87" name="OpenSolver10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EAFAF528-D3EA-4583-BE24-44E0B28C2A82}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C6AC16B-5E9E-4926-8F6A-0D29875EDAE5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4946,10 +4952,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="12" name="OpenSolver11">
+        <xdr:cNvPr id="88" name="OpenSolver11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC61168E-A26F-4571-8355-7EC8AF4EA530}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{209CE62E-9836-4BEF-84BA-D04C5E3D079F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5028,10 +5034,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="13" name="OpenSolver12">
+        <xdr:cNvPr id="89" name="OpenSolver12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7AC7CE0E-792E-4D11-BD88-34EF910388AF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9898B303-1B8A-4C15-97D6-7767114BABA4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5113,16 +5119,16 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="14" name="OpenSolver13">
+        <xdr:cNvPr id="90" name="OpenSolver13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD4A989D-03B0-40E1-9E26-3D9DC85152CA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{453A05F1-E5E0-4395-A4C0-97AAFB1090F2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="12" idx="3"/>
-          <a:endCxn id="13" idx="1"/>
+          <a:stCxn id="88" idx="3"/>
+          <a:endCxn id="89" idx="1"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -5174,10 +5180,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="15" name="OpenSolver14">
+        <xdr:cNvPr id="91" name="OpenSolver14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{116EA6F6-067E-45B5-BC9D-B650EF601F0A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5CDD051E-8482-4CF1-965E-33F29246E2BE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5261,10 +5267,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="16" name="OpenSolver15">
+        <xdr:cNvPr id="92" name="OpenSolver15">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{215AAE4F-27A4-440A-8985-45DA37E4AA16}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D80B1B14-3A03-4BC2-9261-8C74E73634C0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5343,10 +5349,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="17" name="OpenSolver16">
+        <xdr:cNvPr id="93" name="OpenSolver16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A449F3B6-DC8A-4DD8-A641-E8907449AC5C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F4655F56-9469-416C-B2B2-96084DAD59E5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5428,16 +5434,16 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="18" name="OpenSolver17">
+        <xdr:cNvPr id="94" name="OpenSolver17">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FDE5B852-01D7-4D40-A9C0-60734C7A01C7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6092337C-4774-4D1F-A1FF-35247999F96E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="16" idx="3"/>
-          <a:endCxn id="17" idx="1"/>
+          <a:stCxn id="92" idx="3"/>
+          <a:endCxn id="93" idx="1"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -5489,10 +5495,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="19" name="OpenSolver18">
+        <xdr:cNvPr id="95" name="OpenSolver18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2F7A74BB-3ED5-47DB-805A-C517A1FAEEC1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81581D8C-B245-4DD5-9F4B-5A9648C3B392}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5576,10 +5582,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="20" name="OpenSolver19">
+        <xdr:cNvPr id="96" name="OpenSolver19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41F50D52-044B-425E-A106-686EE3A022B9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5CEBA30-06F2-4F5B-B472-18CC2CF4BCA5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5658,10 +5664,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="21" name="OpenSolver20">
+        <xdr:cNvPr id="97" name="OpenSolver20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9BBB9194-7FB2-40D7-8485-D34B2AC3418A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F48FB8E4-3AF6-42E3-B3CB-D8FEA96C9035}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5743,16 +5749,16 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="22" name="OpenSolver21">
+        <xdr:cNvPr id="98" name="OpenSolver21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B38BBF25-E786-49C9-B5CD-DA7B88D51C9F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F861840B-CE2B-41B0-8A3D-DAFED86629AA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="20" idx="3"/>
-          <a:endCxn id="21" idx="1"/>
+          <a:stCxn id="96" idx="3"/>
+          <a:endCxn id="97" idx="1"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -5804,10 +5810,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="23" name="OpenSolver22">
+        <xdr:cNvPr id="99" name="OpenSolver22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{36A90B40-9C85-4A28-9860-75128B4E2C62}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B0E82737-08DA-446C-842E-7894EA982429}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5891,10 +5897,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="24" name="OpenSolver23">
+        <xdr:cNvPr id="100" name="OpenSolver23">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{91CBF10F-09FC-4CB4-80A7-12316C64D980}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{760B8027-7349-430E-B010-C15F61AF4715}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5973,10 +5979,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="25" name="OpenSolver24">
+        <xdr:cNvPr id="101" name="OpenSolver24">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC2D3FED-376E-40BA-9AFE-B7C95122E34D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED2FA4B2-3F2A-4D83-BC91-EDA50F8BB0A5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6058,16 +6064,16 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="26" name="OpenSolver25">
+        <xdr:cNvPr id="102" name="OpenSolver25">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7FE66ABD-1C29-4F68-9414-D260530EFFAC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E6A58FD4-6EAE-4B35-AA76-6BDFE590E5B8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="24" idx="3"/>
-          <a:endCxn id="25" idx="1"/>
+          <a:stCxn id="100" idx="3"/>
+          <a:endCxn id="101" idx="1"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -6119,10 +6125,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="27" name="OpenSolver26">
+        <xdr:cNvPr id="103" name="OpenSolver26">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A6116E2-110A-4285-8ABC-7DF45AF87EC5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89803477-9F71-4F39-AE30-E10CA4B04305}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6206,10 +6212,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="28" name="OpenSolver27">
+        <xdr:cNvPr id="104" name="OpenSolver27">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{11C30E3F-0598-4FCC-BAFC-0BF06945FAA6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6280D681-F93F-4AC6-B4A3-A14490A9B231}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6288,10 +6294,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="29" name="OpenSolver28">
+        <xdr:cNvPr id="105" name="OpenSolver28">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1E25E00-BE42-4D74-B518-94596EFA4AD0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A6081EE9-C81F-434D-B417-0BFEB682EC8D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6373,16 +6379,16 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="30" name="OpenSolver29">
+        <xdr:cNvPr id="106" name="OpenSolver29">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D209F7A-F1FE-40FA-81A6-9D0BAF32CDB7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{44B38B33-09B5-4D5A-87FF-64F88FBB83A7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="28" idx="3"/>
-          <a:endCxn id="29" idx="1"/>
+          <a:stCxn id="104" idx="3"/>
+          <a:endCxn id="105" idx="1"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -6434,10 +6440,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="31" name="OpenSolver30">
+        <xdr:cNvPr id="107" name="OpenSolver30">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25E03FF5-E0D3-4153-AF9F-0401F6165760}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B8E786BE-8ED7-40B5-AB56-5B01F4CAE9CD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6447,6 +6453,321 @@
         <a:xfrm>
           <a:off x="21027391" y="12499340"/>
           <a:ext cx="381000" cy="254000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:noFill/>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="12700" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:miter lim="800000"/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="tr-TR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>198119</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>198119</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="108" name="OpenSolver31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A2C1F76-F79B-4113-AE4F-D38155647CD8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14622780" y="14112239"/>
+          <a:ext cx="617220" cy="990600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="CC0099"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="25400" tIns="25400" rIns="0" bIns="0" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="tr-TR" sz="1100" b="1">
+            <a:solidFill>
+              <a:srgbClr val="CC0099"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>198119</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>198119</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="109" name="OpenSolver32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3108B472-69A1-4FFE-80CB-6E9DBB75CD9A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15925800" y="14112239"/>
+          <a:ext cx="617220" cy="990600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="CC0099"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="25400" tIns="25400" rIns="0" bIns="0" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="tr-TR" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="CC0099"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>=</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>99059</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>99059</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="110" name="OpenSolver33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0200D30D-255E-48FE-8CC6-BDEDDDAA403B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="108" idx="3"/>
+          <a:endCxn id="109" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15240000" y="14607539"/>
+          <a:ext cx="685800" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:srgbClr val="CC0099"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:headEnd type="none"/>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>170179</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>27939</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="111" name="OpenSolver34">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF995997-BE07-4B79-9153-7FC7947C6420}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15489382" y="14218688"/>
+          <a:ext cx="381000" cy="245687"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6521,10 +6842,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="32" name="OpenSolver31">
+        <xdr:cNvPr id="112" name="OpenSolver35">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5AEE190A-8529-4EFF-A854-23BD6DFDEE08}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A50E7DD-D84F-47E2-B8F5-36D00EA3B71F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6603,10 +6924,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="33" name="OpenSolver32">
+        <xdr:cNvPr id="113" name="OpenSolver36">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{26C12812-B8F8-4348-946B-41330610C09C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3DD1D675-273E-49AD-B1EF-CB44C4D24830}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6696,10 +7017,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="34" name="OpenSolver33">
+        <xdr:cNvPr id="114" name="OpenSolver37">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB455ADE-D2E8-4881-A009-D2C20004E899}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F828920-99BD-4060-ABB9-210FA60B079C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6778,10 +7099,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="35" name="OpenSolver34">
+        <xdr:cNvPr id="115" name="OpenSolver38">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62ED9C17-7F4A-4111-BD59-AD7B2890FCF5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99DC5434-0ACA-4BED-9D4F-6D2350D112EE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6871,10 +7192,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="36" name="OpenSolver35">
+        <xdr:cNvPr id="116" name="OpenSolver39">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99B86859-543E-4C57-A65D-7B2AD3D057F7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B784EA4-6E04-42BF-A9D5-AD91B71FC08F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6953,10 +7274,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="37" name="OpenSolver36">
+        <xdr:cNvPr id="117" name="OpenSolver40">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED81621D-C155-40D3-9DEF-826284C42951}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4E397ADA-0F65-4C4C-B290-A736D810958B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7046,10 +7367,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="38" name="OpenSolver37">
+        <xdr:cNvPr id="118" name="OpenSolver41">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{939DA02F-DE2C-4A96-8A15-3B45BA732D1D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D6257EF-8C83-421F-B7DA-5DAC2DBC5246}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7128,10 +7449,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="39" name="OpenSolver38">
+        <xdr:cNvPr id="119" name="OpenSolver42">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9B7FCE64-791C-4F55-8AC7-022D38C13F78}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4BE3D936-27D7-4D61-8F8F-60339FCABCC9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7512,7 +7833,7 @@
       <selection activeCell="B6" sqref="B6:H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5.77734375" style="56" customWidth="1"/>
     <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
@@ -7524,12 +7845,12 @@
     <col min="8" max="8" width="17.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A1" s="56" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A2" s="56" t="s">
         <v>41</v>
       </c>
@@ -7541,7 +7862,7 @@
       <c r="G2" s="46"/>
       <c r="H2" s="46"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A3" s="56" t="s">
         <v>1160</v>
       </c>
@@ -7553,7 +7874,7 @@
       <c r="G3" s="46"/>
       <c r="H3" s="46"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="B4" s="46"/>
       <c r="C4" s="46"/>
       <c r="D4" s="46"/>
@@ -7597,7 +7918,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="B7" s="47" t="s">
         <v>50</v>
       </c>
@@ -7618,7 +7939,7 @@
         <v>1E+100</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="B8" s="47" t="s">
         <v>51</v>
       </c>
@@ -7639,7 +7960,7 @@
         <v>1E+100</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="B9" s="47" t="s">
         <v>52</v>
       </c>
@@ -7660,7 +7981,7 @@
         <v>1E+100</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="B10" s="47" t="s">
         <v>53</v>
       </c>
@@ -7681,7 +8002,7 @@
         <v>1E+100</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="B11" s="47" t="s">
         <v>54</v>
       </c>
@@ -7702,7 +8023,7 @@
         <v>1E+100</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="B12" s="47" t="s">
         <v>55</v>
       </c>
@@ -7723,7 +8044,7 @@
         <v>1E+100</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="B13" s="47" t="s">
         <v>56</v>
       </c>
@@ -7744,7 +8065,7 @@
         <v>1E+100</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="B14" s="47" t="s">
         <v>57</v>
       </c>
@@ -7765,7 +8086,7 @@
         <v>1E+100</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="B15" s="47" t="s">
         <v>58</v>
       </c>
@@ -7786,7 +8107,7 @@
         <v>1E+100</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="B16" s="47" t="s">
         <v>59</v>
       </c>
@@ -7807,7 +8128,7 @@
         <v>1E+100</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:8" ht="15" x14ac:dyDescent="0.3">
       <c r="B17" s="47" t="s">
         <v>60</v>
       </c>
@@ -7828,7 +8149,7 @@
         <v>1E+100</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:8" ht="15" x14ac:dyDescent="0.3">
       <c r="B18" s="47" t="s">
         <v>61</v>
       </c>
@@ -7849,7 +8170,7 @@
         <v>1E+100</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:8" ht="15" x14ac:dyDescent="0.3">
       <c r="B19" s="47" t="s">
         <v>62</v>
       </c>
@@ -7870,7 +8191,7 @@
         <v>1E+100</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:8" ht="15" x14ac:dyDescent="0.3">
       <c r="B20" s="47" t="s">
         <v>63</v>
       </c>
@@ -7891,7 +8212,7 @@
         <v>1E+100</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:8" ht="15" x14ac:dyDescent="0.3">
       <c r="B21" s="47" t="s">
         <v>64</v>
       </c>
@@ -7912,7 +8233,7 @@
         <v>1E+100</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:8" ht="15" x14ac:dyDescent="0.3">
       <c r="B22" s="47" t="s">
         <v>65</v>
       </c>
@@ -7933,7 +8254,7 @@
         <v>1E+100</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:8" ht="15" x14ac:dyDescent="0.3">
       <c r="B23" s="47" t="s">
         <v>66</v>
       </c>
@@ -7954,7 +8275,7 @@
         <v>1E+100</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:8" ht="15" x14ac:dyDescent="0.3">
       <c r="B24" s="47" t="s">
         <v>67</v>
       </c>
@@ -7975,7 +8296,7 @@
         <v>1E+100</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:8" ht="15" x14ac:dyDescent="0.3">
       <c r="B25" s="47" t="s">
         <v>68</v>
       </c>
@@ -7996,7 +8317,7 @@
         <v>1E+100</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:8" ht="15" x14ac:dyDescent="0.3">
       <c r="B26" s="47" t="s">
         <v>69</v>
       </c>
@@ -8017,7 +8338,7 @@
         <v>1E+100</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:8" ht="15" x14ac:dyDescent="0.3">
       <c r="B27" s="47" t="s">
         <v>70</v>
       </c>
@@ -8038,7 +8359,7 @@
         <v>1E+100</v>
       </c>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:8" ht="15" x14ac:dyDescent="0.3">
       <c r="B28" s="47" t="s">
         <v>71</v>
       </c>
@@ -18076,7 +18397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="506" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="506" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B506" s="50" t="s">
         <v>549</v>
       </c>
@@ -18106,7 +18427,7 @@
       <c r="G507" s="46"/>
       <c r="H507" s="46"/>
     </row>
-    <row r="508" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="508" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A508" s="56" t="s">
         <v>550</v>
       </c>
@@ -18118,7 +18439,7 @@
       <c r="G508" s="46"/>
       <c r="H508" s="46"/>
     </row>
-    <row r="509" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="509" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B509" s="53" t="s">
         <v>43</v>
       </c>
@@ -31895,7 +32216,7 @@
         <v>0.70698916050000005</v>
       </c>
     </row>
-    <row r="1108" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1108" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1108" s="50" t="s">
         <v>1159</v>
       </c>
@@ -31937,11 +32258,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7930316F-CD20-49E5-A6A0-4C42FB60CBBA}">
   <dimension ref="A1:CM132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="112" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AB64" sqref="AB64"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="S53" sqref="S53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.44140625" style="1" bestFit="1" customWidth="1"/>
@@ -31983,7 +32304,7 @@
     <col min="70" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:81" ht="16.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:81" ht="16.350000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="38"/>
       <c r="C1" s="38"/>
       <c r="D1" s="38"/>
@@ -32003,7 +32324,7 @@
       <c r="R1" s="38"/>
       <c r="S1" s="38"/>
     </row>
-    <row r="2" spans="2:81" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:81" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
@@ -32089,7 +32410,7 @@
       <c r="CB2" s="3"/>
       <c r="CC2" s="5"/>
     </row>
-    <row r="3" spans="2:81" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:81" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B3" s="7"/>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
@@ -32175,7 +32496,7 @@
       <c r="CB3" s="8"/>
       <c r="CC3" s="9"/>
     </row>
-    <row r="4" spans="2:81" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:81" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B4" s="7"/>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
@@ -32272,7 +32593,7 @@
       <c r="CB4" s="8"/>
       <c r="CC4" s="9"/>
     </row>
-    <row r="5" spans="2:81" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:81" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B5" s="13"/>
       <c r="C5" s="11" t="s">
         <v>9</v>
@@ -32462,7 +32783,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:81" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:81" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B6" s="41">
         <v>1</v>
       </c>
@@ -32552,7 +32873,7 @@
         <v>0</v>
       </c>
       <c r="AL6" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM6" s="16">
         <v>0</v>
@@ -32562,7 +32883,7 @@
         <v>1</v>
       </c>
       <c r="AP6" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ6" s="16">
         <v>0</v>
@@ -32619,7 +32940,7 @@
       </c>
       <c r="BK6" s="16">
         <f>AI6+AP6+AW6+BD6</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BL6" s="16">
         <f t="shared" ref="BL6:BO6" si="0">AJ6+AQ6+AX6+BE6</f>
@@ -32631,7 +32952,7 @@
       </c>
       <c r="BN6" s="16">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BO6" s="16">
         <f t="shared" si="0"/>
@@ -32643,7 +32964,7 @@
       </c>
       <c r="BR6" s="16">
         <f>AI6+AP6*2+AW6*3+BD6*4</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BS6" s="16">
         <f t="shared" ref="BS6:BV6" si="1">AJ6+AQ6*2+AX6*3+BE6*4</f>
@@ -32655,7 +32976,7 @@
       </c>
       <c r="BU6" s="16">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BV6" s="16">
         <f t="shared" si="1"/>
@@ -32667,7 +32988,7 @@
       </c>
       <c r="BY6" s="16">
         <f>AI6+AP6*POWER(2,$O6)+AW6*POWER(3,$O6)+BD6*POWER(4,$O6)</f>
-        <v>0</v>
+        <v>1.4142135623730951</v>
       </c>
       <c r="BZ6" s="16">
         <f t="shared" ref="BZ6:CC6" si="2">AJ6+AQ6*POWER(2,$O6)+AX6*POWER(3,$O6)+BE6*POWER(4,$O6)</f>
@@ -32679,14 +33000,14 @@
       </c>
       <c r="CB6" s="16">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CC6" s="19">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:81" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:81" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B7" s="41">
         <v>2</v>
       </c>
@@ -32910,7 +33231,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:81" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:81" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B8" s="41">
         <v>3</v>
       </c>
@@ -32994,10 +33315,10 @@
         <v>0</v>
       </c>
       <c r="AJ8" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK8" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL8" s="16">
         <v>0</v>
@@ -33071,11 +33392,11 @@
       </c>
       <c r="BL8" s="16">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BM8" s="16">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BN8" s="16">
         <f t="shared" si="11"/>
@@ -33095,11 +33416,11 @@
       </c>
       <c r="BS8" s="16">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BT8" s="16">
         <f t="shared" si="15"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BU8" s="16">
         <f t="shared" si="16"/>
@@ -33119,11 +33440,11 @@
       </c>
       <c r="BZ8" s="16">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CA8" s="16">
         <f t="shared" si="20"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CB8" s="16">
         <f t="shared" si="21"/>
@@ -33134,7 +33455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:81" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:81" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B9" s="41">
         <v>4</v>
       </c>
@@ -33358,7 +33679,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:81" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:81" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B10" s="41">
         <v>5</v>
       </c>
@@ -33502,10 +33823,10 @@
         <v>0</v>
       </c>
       <c r="BF10" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BG10" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BH10" s="19">
         <v>0</v>
@@ -33523,11 +33844,11 @@
       </c>
       <c r="BM10" s="16">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BN10" s="16">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BO10" s="16">
         <f t="shared" si="12"/>
@@ -33547,11 +33868,11 @@
       </c>
       <c r="BT10" s="16">
         <f t="shared" si="15"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="BU10" s="16">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="BV10" s="16">
         <f t="shared" si="17"/>
@@ -33571,18 +33892,18 @@
       </c>
       <c r="CA10" s="16">
         <f t="shared" si="20"/>
-        <v>3.4822022531844965</v>
+        <v>0</v>
       </c>
       <c r="CB10" s="16">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>3.4822022531844965</v>
       </c>
       <c r="CC10" s="19">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:81" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:81" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B11" s="41">
         <v>6</v>
       </c>
@@ -33663,7 +33984,7 @@
         <v>6</v>
       </c>
       <c r="AI11" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ11" s="16">
         <v>0</v>
@@ -33739,7 +34060,7 @@
       </c>
       <c r="BK11" s="16">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BL11" s="16">
         <f t="shared" si="9"/>
@@ -33763,7 +34084,7 @@
       </c>
       <c r="BR11" s="16">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BS11" s="16">
         <f t="shared" si="14"/>
@@ -33787,7 +34108,7 @@
       </c>
       <c r="BY11" s="16">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BZ11" s="16">
         <f t="shared" si="19"/>
@@ -33806,7 +34127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:81" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:81" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B12" s="41">
         <v>7</v>
       </c>
@@ -33887,7 +34208,7 @@
         <v>7</v>
       </c>
       <c r="AI12" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ12" s="16">
         <v>0</v>
@@ -33963,7 +34284,7 @@
       </c>
       <c r="BK12" s="16">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BL12" s="16">
         <f t="shared" si="9"/>
@@ -33987,7 +34308,7 @@
       </c>
       <c r="BR12" s="16">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BS12" s="16">
         <f t="shared" si="14"/>
@@ -34011,7 +34332,7 @@
       </c>
       <c r="BY12" s="16">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BZ12" s="16">
         <f t="shared" si="19"/>
@@ -34030,7 +34351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:81" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:81" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B13" s="41">
         <v>8</v>
       </c>
@@ -34114,7 +34435,7 @@
         <v>0</v>
       </c>
       <c r="AJ13" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK13" s="16">
         <v>0</v>
@@ -34123,7 +34444,7 @@
         <v>0</v>
       </c>
       <c r="AM13" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN13" s="8"/>
       <c r="AO13" s="23">
@@ -34191,7 +34512,7 @@
       </c>
       <c r="BL13" s="16">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BM13" s="16">
         <f t="shared" si="10"/>
@@ -34203,7 +34524,7 @@
       </c>
       <c r="BO13" s="16">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP13" s="8"/>
       <c r="BQ13" s="23">
@@ -34215,7 +34536,7 @@
       </c>
       <c r="BS13" s="16">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BT13" s="16">
         <f t="shared" si="15"/>
@@ -34227,7 +34548,7 @@
       </c>
       <c r="BV13" s="16">
         <f t="shared" si="17"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BW13" s="8"/>
       <c r="BX13" s="23">
@@ -34239,7 +34560,7 @@
       </c>
       <c r="BZ13" s="16">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CA13" s="16">
         <f t="shared" si="20"/>
@@ -34251,10 +34572,10 @@
       </c>
       <c r="CC13" s="19">
         <f t="shared" si="22"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="2:81" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:81" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B14" s="41">
         <v>9</v>
       </c>
@@ -34357,7 +34678,7 @@
         <v>0</v>
       </c>
       <c r="AQ14" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR14" s="16">
         <v>0</v>
@@ -34376,7 +34697,7 @@
         <v>0</v>
       </c>
       <c r="AX14" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AY14" s="16">
         <v>0</v>
@@ -34439,7 +34760,7 @@
       </c>
       <c r="BS14" s="16">
         <f t="shared" si="14"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="BT14" s="16">
         <f t="shared" si="15"/>
@@ -34463,7 +34784,7 @@
       </c>
       <c r="BZ14" s="16">
         <f t="shared" si="19"/>
-        <v>2.4082246852806923</v>
+        <v>1.7411011265922482</v>
       </c>
       <c r="CA14" s="16">
         <f t="shared" si="20"/>
@@ -34478,7 +34799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:81" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:81" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B15" s="41">
         <v>10</v>
       </c>
@@ -34597,7 +34918,7 @@
         <v>10</v>
       </c>
       <c r="AW15" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AX15" s="16">
         <v>0</v>
@@ -34609,7 +34930,7 @@
         <v>0</v>
       </c>
       <c r="BA15" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BB15" s="8"/>
       <c r="BC15" s="23">
@@ -34635,7 +34956,7 @@
       </c>
       <c r="BK15" s="16">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BL15" s="16">
         <f t="shared" si="9"/>
@@ -34651,7 +34972,7 @@
       </c>
       <c r="BO15" s="16">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BP15" s="8"/>
       <c r="BQ15" s="23">
@@ -34659,7 +34980,7 @@
       </c>
       <c r="BR15" s="16">
         <f t="shared" si="13"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BS15" s="16">
         <f t="shared" si="14"/>
@@ -34675,7 +34996,7 @@
       </c>
       <c r="BV15" s="16">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BW15" s="8"/>
       <c r="BX15" s="23">
@@ -34683,7 +35004,7 @@
       </c>
       <c r="BY15" s="16">
         <f t="shared" si="18"/>
-        <v>2.4082246852806923</v>
+        <v>0</v>
       </c>
       <c r="BZ15" s="16">
         <f t="shared" si="19"/>
@@ -34699,10 +35020,10 @@
       </c>
       <c r="CC15" s="19">
         <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="2:81" x14ac:dyDescent="0.3">
+        <v>2.4082246852806923</v>
+      </c>
+    </row>
+    <row r="16" spans="2:81" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B16" s="41">
         <v>11</v>
       </c>
@@ -34789,13 +35110,13 @@
         <v>0</v>
       </c>
       <c r="AK16" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL16" s="16">
         <v>0</v>
       </c>
       <c r="AM16" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN16" s="8"/>
       <c r="AO16" s="23">
@@ -34867,7 +35188,7 @@
       </c>
       <c r="BM16" s="16">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BN16" s="16">
         <f t="shared" si="11"/>
@@ -34875,7 +35196,7 @@
       </c>
       <c r="BO16" s="16">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BP16" s="8"/>
       <c r="BQ16" s="23">
@@ -34891,7 +35212,7 @@
       </c>
       <c r="BT16" s="16">
         <f t="shared" si="15"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BU16" s="16">
         <f t="shared" si="16"/>
@@ -34899,7 +35220,7 @@
       </c>
       <c r="BV16" s="16">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BW16" s="8"/>
       <c r="BX16" s="23">
@@ -34915,7 +35236,7 @@
       </c>
       <c r="CA16" s="16">
         <f t="shared" si="20"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CB16" s="16">
         <f t="shared" si="21"/>
@@ -34923,10 +35244,10 @@
       </c>
       <c r="CC16" s="19">
         <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:81" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:81" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B17" s="41">
         <v>12</v>
       </c>
@@ -35150,7 +35471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:81" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:81" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B18" s="41">
         <v>13</v>
       </c>
@@ -35243,7 +35564,7 @@
         <v>0</v>
       </c>
       <c r="AM18" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN18" s="8"/>
       <c r="AO18" s="23">
@@ -35323,7 +35644,7 @@
       </c>
       <c r="BO18" s="16">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BP18" s="8"/>
       <c r="BQ18" s="23">
@@ -35347,7 +35668,7 @@
       </c>
       <c r="BV18" s="16">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BW18" s="8"/>
       <c r="BX18" s="23">
@@ -35371,10 +35692,10 @@
       </c>
       <c r="CC18" s="19">
         <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:81" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:81" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B19" s="41">
         <v>14</v>
       </c>
@@ -35598,7 +35919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:81" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:81" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B20" s="41">
         <v>15</v>
       </c>
@@ -35822,7 +36143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:81" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:81" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B21" s="41">
         <v>16</v>
       </c>
@@ -36046,7 +36367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:81" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:81" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B22" s="41">
         <v>17</v>
       </c>
@@ -36270,7 +36591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:81" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:81" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B23" s="41">
         <v>18</v>
       </c>
@@ -36494,7 +36815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:81" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:81" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B24" s="41">
         <v>19</v>
       </c>
@@ -36575,7 +36896,7 @@
         <v>19</v>
       </c>
       <c r="AI24" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ24" s="16">
         <v>0</v>
@@ -36651,7 +36972,7 @@
       </c>
       <c r="BK24" s="16">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BL24" s="16">
         <f t="shared" si="9"/>
@@ -36675,7 +36996,7 @@
       </c>
       <c r="BR24" s="16">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BS24" s="16">
         <f t="shared" si="14"/>
@@ -36699,7 +37020,7 @@
       </c>
       <c r="BY24" s="16">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BZ24" s="16">
         <f t="shared" si="19"/>
@@ -36718,7 +37039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:81" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:81" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B25" s="41">
         <v>20</v>
       </c>
@@ -36942,7 +37263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:81" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:81" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B26" s="41">
         <v>21</v>
       </c>
@@ -37032,7 +37353,7 @@
         <v>0</v>
       </c>
       <c r="AL26" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM26" s="16">
         <v>0</v>
@@ -37073,7 +37394,7 @@
         <v>0</v>
       </c>
       <c r="BA26" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB26" s="8"/>
       <c r="BC26" s="23">
@@ -37111,11 +37432,11 @@
       </c>
       <c r="BN26" s="16">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BO26" s="16">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP26" s="8"/>
       <c r="BQ26" s="23">
@@ -37135,11 +37456,11 @@
       </c>
       <c r="BU26" s="16">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BV26" s="16">
         <f t="shared" si="17"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BW26" s="8"/>
       <c r="BX26" s="23">
@@ -37159,14 +37480,14 @@
       </c>
       <c r="CB26" s="16">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CC26" s="19">
         <f t="shared" si="22"/>
-        <v>1.9331820449317627</v>
-      </c>
-    </row>
-    <row r="27" spans="2:81" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:81" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B27" s="41">
         <v>22</v>
       </c>
@@ -37247,7 +37568,7 @@
         <v>22</v>
       </c>
       <c r="AI27" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ27" s="16">
         <v>0</v>
@@ -37256,7 +37577,7 @@
         <v>0</v>
       </c>
       <c r="AL27" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM27" s="16">
         <v>0</v>
@@ -37323,7 +37644,7 @@
       </c>
       <c r="BK27" s="16">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BL27" s="16">
         <f t="shared" si="9"/>
@@ -37335,7 +37656,7 @@
       </c>
       <c r="BN27" s="16">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BO27" s="16">
         <f t="shared" si="12"/>
@@ -37347,7 +37668,7 @@
       </c>
       <c r="BR27" s="16">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BS27" s="16">
         <f t="shared" si="14"/>
@@ -37359,7 +37680,7 @@
       </c>
       <c r="BU27" s="16">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BV27" s="16">
         <f t="shared" si="17"/>
@@ -37371,7 +37692,7 @@
       </c>
       <c r="BY27" s="16">
         <f t="shared" si="18"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BZ27" s="16">
         <f t="shared" si="19"/>
@@ -37383,14 +37704,14 @@
       </c>
       <c r="CB27" s="16">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CC27" s="19">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:81" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:81" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B28" s="41">
         <v>23</v>
       </c>
@@ -37614,7 +37935,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="2:81" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:81" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B29" s="41">
         <v>24</v>
       </c>
@@ -37707,7 +38028,7 @@
         <v>0</v>
       </c>
       <c r="AM29" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN29" s="8"/>
       <c r="AO29" s="23">
@@ -37726,7 +38047,7 @@
         <v>0</v>
       </c>
       <c r="AT29" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AU29" s="8"/>
       <c r="AV29" s="23">
@@ -37811,7 +38132,7 @@
       </c>
       <c r="BV29" s="16">
         <f t="shared" si="17"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BW29" s="8"/>
       <c r="BX29" s="23">
@@ -37835,10 +38156,10 @@
       </c>
       <c r="CC29" s="19">
         <f t="shared" si="22"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="2:81" x14ac:dyDescent="0.3">
+        <v>1.7411011265922482</v>
+      </c>
+    </row>
+    <row r="30" spans="2:81" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B30" s="41">
         <v>25</v>
       </c>
@@ -37963,7 +38284,7 @@
         <v>0</v>
       </c>
       <c r="AY30" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AZ30" s="16">
         <v>0</v>
@@ -37985,7 +38306,7 @@
         <v>0</v>
       </c>
       <c r="BG30" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BH30" s="19">
         <v>0</v>
@@ -38003,11 +38324,11 @@
       </c>
       <c r="BM30" s="16">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BN30" s="16">
         <f t="shared" si="11"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BO30" s="16">
         <f t="shared" si="12"/>
@@ -38027,11 +38348,11 @@
       </c>
       <c r="BT30" s="16">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BU30" s="16">
         <f t="shared" si="16"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="BV30" s="16">
         <f t="shared" si="17"/>
@@ -38051,18 +38372,18 @@
       </c>
       <c r="CA30" s="16">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>2.6878753795222869</v>
       </c>
       <c r="CB30" s="16">
         <f t="shared" si="21"/>
-        <v>3.4822022531844965</v>
+        <v>0</v>
       </c>
       <c r="CC30" s="19">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:81" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:81" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B31" s="7"/>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
@@ -38244,7 +38565,7 @@
       <c r="CB32" s="8"/>
       <c r="CC32" s="9"/>
     </row>
-    <row r="33" spans="2:81" ht="16.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:81" ht="16.350000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B33" s="41">
         <v>1</v>
       </c>
@@ -38336,7 +38657,7 @@
       <c r="CB33" s="26"/>
       <c r="CC33" s="27"/>
     </row>
-    <row r="34" spans="2:81" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:81" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B34" s="41">
         <v>2</v>
       </c>
@@ -38401,7 +38722,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="2:81" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:81" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B35" s="41">
         <v>3</v>
       </c>
@@ -38473,7 +38794,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="36" spans="2:81" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:81" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B36" s="41">
         <v>4</v>
       </c>
@@ -38518,7 +38839,7 @@
       <c r="AE36" s="8"/>
       <c r="AF36" s="9"/>
     </row>
-    <row r="37" spans="2:81" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:81" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B37" s="41">
         <v>5</v>
       </c>
@@ -38563,7 +38884,7 @@
       <c r="AE37" s="8"/>
       <c r="AF37" s="9"/>
     </row>
-    <row r="38" spans="2:81" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:81" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B38" s="32"/>
       <c r="C38" s="28"/>
       <c r="D38" s="8"/>
@@ -38596,7 +38917,7 @@
       <c r="AE38" s="8"/>
       <c r="AF38" s="9"/>
     </row>
-    <row r="39" spans="2:81" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:81" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B39" s="7"/>
       <c r="C39" s="8"/>
       <c r="D39" s="8"/>
@@ -38629,7 +38950,7 @@
       <c r="AE39" s="8"/>
       <c r="AF39" s="9"/>
     </row>
-    <row r="40" spans="2:81" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:81" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B40" s="7"/>
       <c r="C40" s="8"/>
       <c r="D40" s="8"/>
@@ -38662,7 +38983,7 @@
       <c r="AE40" s="8"/>
       <c r="AF40" s="9"/>
     </row>
-    <row r="41" spans="2:81" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:81" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B41" s="10" t="s">
         <v>19</v>
       </c>
@@ -38697,7 +39018,7 @@
       <c r="AE41" s="8"/>
       <c r="AF41" s="9"/>
     </row>
-    <row r="42" spans="2:81" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:81" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B42" s="7">
         <v>2</v>
       </c>
@@ -38734,7 +39055,7 @@
       <c r="AE42" s="8"/>
       <c r="AF42" s="9"/>
     </row>
-    <row r="43" spans="2:81" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:81" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B43" s="7">
         <v>16</v>
       </c>
@@ -38771,7 +39092,7 @@
       <c r="AE43" s="8"/>
       <c r="AF43" s="9"/>
     </row>
-    <row r="44" spans="2:81" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:81" ht="15.75" x14ac:dyDescent="0.3">
       <c r="D44" s="8"/>
       <c r="E44" s="8"/>
       <c r="F44" s="8"/>
@@ -38802,7 +39123,7 @@
       <c r="AE44" s="8"/>
       <c r="AF44" s="9"/>
     </row>
-    <row r="45" spans="2:81" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:81" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B45" s="7"/>
       <c r="C45" s="8"/>
       <c r="D45" s="8"/>
@@ -38835,7 +39156,7 @@
       <c r="AE45" s="8"/>
       <c r="AF45" s="9"/>
     </row>
-    <row r="46" spans="2:81" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:81" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B46" s="10" t="s">
         <v>20</v>
       </c>
@@ -38870,7 +39191,7 @@
       <c r="AE46" s="8"/>
       <c r="AF46" s="9"/>
     </row>
-    <row r="47" spans="2:81" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:81" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B47" s="7">
         <v>1</v>
       </c>
@@ -38907,7 +39228,7 @@
       <c r="AE47" s="8"/>
       <c r="AF47" s="9"/>
     </row>
-    <row r="48" spans="2:81" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:81" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B48" s="7">
         <v>3</v>
       </c>
@@ -38947,7 +39268,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="49" spans="1:91" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:91" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B49" s="7">
         <v>9</v>
       </c>
@@ -38988,7 +39309,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="50" spans="1:91" ht="16.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:91" ht="16.350000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B50" s="25">
         <v>16</v>
       </c>
@@ -39029,13 +39350,13 @@
         <v>99</v>
       </c>
     </row>
-    <row r="51" spans="1:91" ht="16.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:91" ht="16.350000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="AH51" s="1">
         <f ca="1">SUM(INDIRECT(ADDRESS(6,26+ROWS($A$1:A3))):INDIRECT(ADDRESS(30,26+ROWS($A$1:A3))))</f>
         <v>78</v>
       </c>
     </row>
-    <row r="52" spans="1:91" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:91" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B52" s="2" t="s">
         <v>5</v>
       </c>
@@ -39053,7 +39374,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="53" spans="1:91" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:91" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B53" s="7"/>
       <c r="C53" s="8"/>
       <c r="D53" s="8"/>
@@ -39069,7 +39390,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="54" spans="1:91" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:91" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B54" s="7"/>
       <c r="C54" s="8"/>
       <c r="D54" s="8"/>
@@ -39081,10 +39402,10 @@
       <c r="I54" s="11"/>
       <c r="J54" s="34"/>
     </row>
-    <row r="55" spans="1:91" ht="16.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:91" ht="16.350000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B55" s="25" cm="1">
         <f t="array" ref="B55">SUMPRODUCT(MMULT(BY6:CC30*C6:C30*L6:L30*POWER(F6:F30,O6:O30),I33:I37))</f>
-        <v>6938.3490468496238</v>
+        <v>6737.7151160257772</v>
       </c>
       <c r="C55" s="26"/>
       <c r="D55" s="26"/>
@@ -39096,8 +39417,8 @@
       <c r="I55" s="26"/>
       <c r="J55" s="27"/>
     </row>
-    <row r="56" spans="1:91" ht="16.399999999999999" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="57" spans="1:91" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:91" ht="16.350000000000001" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="57" spans="1:91" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B57" s="2" t="s">
         <v>6</v>
       </c>
@@ -39191,7 +39512,7 @@
       <c r="CL57" s="8"/>
       <c r="CM57" s="8"/>
     </row>
-    <row r="58" spans="1:91" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:91" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B58" s="7"/>
       <c r="C58" s="8"/>
       <c r="D58" s="8"/>
@@ -39283,7 +39604,7 @@
       <c r="CL58" s="8"/>
       <c r="CM58" s="8"/>
     </row>
-    <row r="59" spans="1:91" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:91" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B59" s="7"/>
       <c r="C59" s="8"/>
       <c r="D59" s="8"/>
@@ -39375,7 +39696,7 @@
       <c r="CL59" s="8"/>
       <c r="CM59" s="8"/>
     </row>
-    <row r="60" spans="1:91" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:91" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A60" s="8"/>
       <c r="B60" s="7"/>
       <c r="C60" s="8"/>
@@ -39468,7 +39789,7 @@
       <c r="CL60" s="8"/>
       <c r="CM60" s="8"/>
     </row>
-    <row r="61" spans="1:91" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:91" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A61" s="8"/>
       <c r="B61" s="7"/>
       <c r="C61" s="8"/>
@@ -39561,7 +39882,7 @@
       <c r="CL61" s="8"/>
       <c r="CM61" s="8"/>
     </row>
-    <row r="62" spans="1:91" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:91" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A62" s="8"/>
       <c r="B62" s="7" t="s">
         <v>22</v>
@@ -39666,7 +39987,7 @@
       <c r="CL62" s="8"/>
       <c r="CM62" s="8"/>
     </row>
-    <row r="63" spans="1:91" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:91" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A63" s="8"/>
       <c r="B63" s="7"/>
       <c r="C63" s="8">
@@ -39683,7 +40004,7 @@
       <c r="G63" s="8"/>
       <c r="H63" s="8" cm="1">
         <f t="array" ref="H63">SUM(AA6:AE6*BR6:BV6-R6*BK6:BO6)</f>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="I63" s="8" t="s">
         <v>25</v>
@@ -39695,7 +40016,7 @@
       <c r="L63" s="8"/>
       <c r="M63" s="8" cm="1">
         <f t="array" ref="M63">SUM(AA6:AE6*BR6:BV6-U6*BK6:BO6)</f>
-        <v>-12</v>
+        <v>-7</v>
       </c>
       <c r="N63" s="8" t="s">
         <v>21</v>
@@ -39707,7 +40028,7 @@
       <c r="Q63" s="8"/>
       <c r="R63" s="8" cm="1">
         <f t="array" aca="1" ref="R63" ca="1">-C33+SUM(INDIRECT(ADDRESS(6,69+ROWS($A$1:A1))):INDIRECT(ADDRESS(30,69+ROWS($A$1:A1)))*$F$6:$F$30)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="S63" s="8" t="s">
         <v>21</v>
@@ -39739,11 +40060,11 @@
       </c>
       <c r="AD63" s="8" cm="1">
         <f t="array" aca="1" ref="AD63" ca="1">INDIRECT(ADDRESS(5+$B42,62+COLUMNS($A1:C1)))+INDIRECT(ADDRESS(5+$C42,62+COLUMNS($A1:C1)))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE63" s="8" cm="1">
         <f t="array" aca="1" ref="AE63" ca="1">INDIRECT(ADDRESS(5+$B42,62+COLUMNS($A1:D1)))+INDIRECT(ADDRESS(5+$C42,62+COLUMNS($A1:D1)))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF63" s="8" cm="1">
         <f t="array" aca="1" ref="AF63" ca="1">INDIRECT(ADDRESS(5+$B42,62+COLUMNS($A1:E1)))+INDIRECT(ADDRESS(5+$C42,62+COLUMNS($A1:E1)))</f>
@@ -39821,7 +40142,7 @@
       <c r="CL63" s="8"/>
       <c r="CM63" s="8"/>
     </row>
-    <row r="64" spans="1:91" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:91" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A64" s="8"/>
       <c r="B64" s="7"/>
       <c r="C64" s="8">
@@ -39862,7 +40183,7 @@
       <c r="Q64" s="8"/>
       <c r="R64" s="8" cm="1">
         <f t="array" aca="1" ref="R64" ca="1">-C34+SUM(INDIRECT(ADDRESS(6,69+ROWS($A$1:A2))):INDIRECT(ADDRESS(30,69+ROWS($A$1:A2)))*$F$6:$F$30)</f>
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="S64" s="8" t="s">
         <v>21</v>
@@ -39951,7 +40272,7 @@
       <c r="CL64" s="8"/>
       <c r="CM64" s="8"/>
     </row>
-    <row r="65" spans="1:91" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:91" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A65" s="8"/>
       <c r="B65" s="7"/>
       <c r="C65" s="8">
@@ -39968,7 +40289,7 @@
       <c r="G65" s="8"/>
       <c r="H65" s="8" cm="1">
         <f t="array" ref="H65">SUM(AA8:AE8*BR8:BV8-R8*BK8:BO8)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I65" s="8" t="s">
         <v>25</v>
@@ -39980,7 +40301,7 @@
       <c r="L65" s="8"/>
       <c r="M65" s="8" cm="1">
         <f t="array" ref="M65">SUM(AA8:AE8*BR8:BV8-U8*BK8:BO8)</f>
-        <v>-21</v>
+        <v>-20</v>
       </c>
       <c r="N65" s="8" t="s">
         <v>21</v>
@@ -40106,7 +40427,7 @@
       <c r="CL65" s="8"/>
       <c r="CM65" s="8"/>
     </row>
-    <row r="66" spans="1:91" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:91" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A66" s="8"/>
       <c r="B66" s="7"/>
       <c r="C66" s="8">
@@ -40234,7 +40555,7 @@
       <c r="CL66" s="8"/>
       <c r="CM66" s="8"/>
     </row>
-    <row r="67" spans="1:91" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:91" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A67" s="8"/>
       <c r="B67" s="7"/>
       <c r="C67" s="8">
@@ -40251,7 +40572,7 @@
       <c r="G67" s="8"/>
       <c r="H67" s="8" cm="1">
         <f t="array" ref="H67">SUM(AA10:AE10*BR10:BV10-R10*BK10:BO10)</f>
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="I67" s="8" t="s">
         <v>25</v>
@@ -40263,7 +40584,7 @@
       <c r="L67" s="8"/>
       <c r="M67" s="8" cm="1">
         <f t="array" ref="M67">SUM(AA10:AE10*BR10:BV10-U10*BK10:BO10)</f>
-        <v>-8</v>
+        <v>-4</v>
       </c>
       <c r="N67" s="8" t="s">
         <v>21</v>
@@ -40275,7 +40596,7 @@
       <c r="Q67" s="8"/>
       <c r="R67" s="8" cm="1">
         <f t="array" aca="1" ref="R67" ca="1">-C37+SUM(INDIRECT(ADDRESS(6,69+ROWS($A$1:A5))):INDIRECT(ADDRESS(30,69+ROWS($A$1:A5)))*$F$6:$F$30)</f>
-        <v>-2</v>
+        <v>-6</v>
       </c>
       <c r="S67" s="8" t="s">
         <v>21</v>
@@ -40355,12 +40676,12 @@
       <c r="CL67" s="8"/>
       <c r="CM67" s="8"/>
     </row>
-    <row r="68" spans="1:91" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:91" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A68" s="8"/>
       <c r="B68" s="10"/>
       <c r="C68" s="8">
         <f t="shared" si="23"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D68" s="8" t="s">
         <v>21</v>
@@ -40372,7 +40693,7 @@
       <c r="G68" s="8"/>
       <c r="H68" s="8" cm="1">
         <f t="array" ref="H68">SUM(AA11:AE11*BR11:BV11-R11*BK11:BO11)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I68" s="8" t="s">
         <v>25</v>
@@ -40384,7 +40705,7 @@
       <c r="L68" s="8"/>
       <c r="M68" s="8" cm="1">
         <f t="array" ref="M68">SUM(AA11:AE11*BR11:BV11-U11*BK11:BO11)</f>
-        <v>0</v>
+        <v>-17</v>
       </c>
       <c r="N68" s="8" t="s">
         <v>21</v>
@@ -40469,12 +40790,12 @@
       <c r="CL68" s="8"/>
       <c r="CM68" s="8"/>
     </row>
-    <row r="69" spans="1:91" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:91" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A69" s="8"/>
       <c r="B69" s="10"/>
       <c r="C69" s="8">
         <f t="shared" si="23"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D69" s="8" t="s">
         <v>21</v>
@@ -40486,7 +40807,7 @@
       <c r="G69" s="8"/>
       <c r="H69" s="8" cm="1">
         <f t="array" ref="H69">SUM(AA12:AE12*BR12:BV12-R12*BK12:BO12)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I69" s="8" t="s">
         <v>25</v>
@@ -40498,7 +40819,7 @@
       <c r="L69" s="8"/>
       <c r="M69" s="8" cm="1">
         <f t="array" ref="M69">SUM(AA12:AE12*BR12:BV12-U12*BK12:BO12)</f>
-        <v>0</v>
+        <v>-6</v>
       </c>
       <c r="N69" s="8" t="s">
         <v>21</v>
@@ -40583,7 +40904,7 @@
       <c r="CL69" s="8"/>
       <c r="CM69" s="8"/>
     </row>
-    <row r="70" spans="1:91" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:91" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A70" s="8"/>
       <c r="B70" s="10"/>
       <c r="C70" s="8">
@@ -40697,7 +41018,7 @@
       <c r="CL70" s="8"/>
       <c r="CM70" s="8"/>
     </row>
-    <row r="71" spans="1:91" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:91" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A71" s="8"/>
       <c r="B71" s="10"/>
       <c r="C71" s="8">
@@ -40714,7 +41035,7 @@
       <c r="G71" s="8"/>
       <c r="H71" s="8" cm="1">
         <f t="array" ref="H71">SUM(AA14:AE14*BR14:BV14-R14*BK14:BO14)</f>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="I71" s="8" t="s">
         <v>25</v>
@@ -40726,7 +41047,7 @@
       <c r="L71" s="8"/>
       <c r="M71" s="8" cm="1">
         <f t="array" ref="M71">SUM(AA14:AE14*BR14:BV14-U14*BK14:BO14)</f>
-        <v>-2</v>
+        <v>-5</v>
       </c>
       <c r="N71" s="8" t="s">
         <v>21</v>
@@ -40740,7 +41061,9 @@
       <c r="S71" s="8"/>
       <c r="T71" s="8"/>
       <c r="U71" s="8"/>
-      <c r="V71" s="8"/>
+      <c r="V71" s="8" t="s">
+        <v>1166</v>
+      </c>
       <c r="W71" s="8"/>
       <c r="X71" s="8"/>
       <c r="Y71" s="8"/>
@@ -40811,7 +41134,7 @@
       <c r="CL71" s="8"/>
       <c r="CM71" s="8"/>
     </row>
-    <row r="72" spans="1:91" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:91" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A72" s="8"/>
       <c r="B72" s="10"/>
       <c r="C72" s="8">
@@ -40855,9 +41178,16 @@
       <c r="T72" s="8"/>
       <c r="U72" s="8"/>
       <c r="V72" s="8"/>
-      <c r="W72" s="8"/>
-      <c r="X72" s="8"/>
-      <c r="Y72" s="8"/>
+      <c r="W72" s="8" cm="1">
+        <f t="array" aca="1" ref="W72" ca="1">INDIRECT(ADDRESS(8,62+ROWS($A$1:A1)))-INDIRECT(ADDRESS(13,62+ROWS($A$1:A1)))</f>
+        <v>0</v>
+      </c>
+      <c r="X72" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y72" s="8">
+        <v>0</v>
+      </c>
       <c r="Z72" s="8"/>
       <c r="AA72" s="8"/>
       <c r="AB72" s="8"/>
@@ -40925,7 +41255,7 @@
       <c r="CL72" s="8"/>
       <c r="CM72" s="8"/>
     </row>
-    <row r="73" spans="1:91" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:91" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A73" s="8"/>
       <c r="B73" s="10"/>
       <c r="C73" s="8">
@@ -40969,9 +41299,16 @@
       <c r="T73" s="8"/>
       <c r="U73" s="8"/>
       <c r="V73" s="8"/>
-      <c r="W73" s="8"/>
-      <c r="X73" s="8"/>
-      <c r="Y73" s="8"/>
+      <c r="W73" s="8" cm="1">
+        <f t="array" aca="1" ref="W73" ca="1">INDIRECT(ADDRESS(8,62+ROWS($A$1:A2)))-INDIRECT(ADDRESS(13,62+ROWS($A$1:A2)))</f>
+        <v>0</v>
+      </c>
+      <c r="X73" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y73" s="8">
+        <v>0</v>
+      </c>
       <c r="Z73" s="8"/>
       <c r="AA73" s="8"/>
       <c r="AB73" s="8"/>
@@ -41039,7 +41376,7 @@
       <c r="CL73" s="8"/>
       <c r="CM73" s="8"/>
     </row>
-    <row r="74" spans="1:91" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:91" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A74" s="8"/>
       <c r="B74" s="10"/>
       <c r="C74" s="8">
@@ -41083,9 +41420,16 @@
       <c r="T74" s="8"/>
       <c r="U74" s="8"/>
       <c r="V74" s="8"/>
-      <c r="W74" s="8"/>
-      <c r="X74" s="8"/>
-      <c r="Y74" s="8"/>
+      <c r="W74" s="8" cm="1">
+        <f t="array" aca="1" ref="W74" ca="1">INDIRECT(ADDRESS(8,62+ROWS($A$1:A3)))-INDIRECT(ADDRESS(13,62+ROWS($A$1:A3)))</f>
+        <v>0</v>
+      </c>
+      <c r="X74" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y74" s="8">
+        <v>0</v>
+      </c>
       <c r="Z74" s="8"/>
       <c r="AA74" s="8"/>
       <c r="AB74" s="8"/>
@@ -41153,11 +41497,11 @@
       <c r="CL74" s="8"/>
       <c r="CM74" s="8"/>
     </row>
-    <row r="75" spans="1:91" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:91" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B75" s="10"/>
       <c r="C75" s="8">
         <f t="shared" si="23"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D75" s="8" t="s">
         <v>21</v>
@@ -41169,7 +41513,7 @@
       <c r="G75" s="8"/>
       <c r="H75" s="8" cm="1">
         <f t="array" ref="H75">SUM(AA18:AE18*BR18:BV18-R18*BK18:BO18)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I75" s="8" t="s">
         <v>25</v>
@@ -41181,7 +41525,7 @@
       <c r="L75" s="8"/>
       <c r="M75" s="8" cm="1">
         <f t="array" ref="M75">SUM(AA18:AE18*BR18:BV18-U18*BK18:BO18)</f>
-        <v>0</v>
+        <v>-8</v>
       </c>
       <c r="N75" s="8" t="s">
         <v>21</v>
@@ -41196,9 +41540,16 @@
       <c r="T75" s="8"/>
       <c r="U75" s="8"/>
       <c r="V75" s="8"/>
-      <c r="W75" s="8"/>
-      <c r="X75" s="8"/>
-      <c r="Y75" s="8"/>
+      <c r="W75" s="8" cm="1">
+        <f t="array" aca="1" ref="W75" ca="1">INDIRECT(ADDRESS(8,62+ROWS($A$1:A4)))-INDIRECT(ADDRESS(13,62+ROWS($A$1:A4)))</f>
+        <v>0</v>
+      </c>
+      <c r="X75" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y75" s="8">
+        <v>0</v>
+      </c>
       <c r="Z75" s="8"/>
       <c r="AA75" s="8"/>
       <c r="AB75" s="8"/>
@@ -41266,7 +41617,7 @@
       <c r="CL75" s="8"/>
       <c r="CM75" s="8"/>
     </row>
-    <row r="76" spans="1:91" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:91" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B76" s="7"/>
       <c r="C76" s="8">
         <f t="shared" si="23"/>
@@ -41309,9 +41660,16 @@
       <c r="T76" s="8"/>
       <c r="U76" s="8"/>
       <c r="V76" s="8"/>
-      <c r="W76" s="8"/>
-      <c r="X76" s="8"/>
-      <c r="Y76" s="8"/>
+      <c r="W76" s="8" cm="1">
+        <f t="array" aca="1" ref="W76" ca="1">INDIRECT(ADDRESS(8,62+ROWS($A$1:A5)))-INDIRECT(ADDRESS(13,62+ROWS($A$1:A5)))</f>
+        <v>0</v>
+      </c>
+      <c r="X76" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y76" s="8">
+        <v>0</v>
+      </c>
       <c r="Z76" s="8"/>
       <c r="AA76" s="8"/>
       <c r="AB76" s="8"/>
@@ -41379,7 +41737,7 @@
       <c r="CL76" s="8"/>
       <c r="CM76" s="8"/>
     </row>
-    <row r="77" spans="1:91" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:91" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B77" s="7"/>
       <c r="C77" s="8">
         <f t="shared" si="23"/>
@@ -41835,7 +42193,7 @@
       <c r="B81" s="7"/>
       <c r="C81" s="8">
         <f t="shared" si="23"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D81" s="8" t="s">
         <v>21</v>
@@ -41847,7 +42205,7 @@
       <c r="G81" s="8"/>
       <c r="H81" s="8" cm="1">
         <f t="array" ref="H81">SUM(AA24:AE24*BR24:BV24-R24*BK24:BO24)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I81" s="8" t="s">
         <v>25</v>
@@ -41859,7 +42217,7 @@
       <c r="L81" s="8"/>
       <c r="M81" s="8" cm="1">
         <f t="array" ref="M81">SUM(AA24:AE24*BR24:BV24-U24*BK24:BO24)</f>
-        <v>0</v>
+        <v>-17</v>
       </c>
       <c r="N81" s="8" t="s">
         <v>21</v>
@@ -42073,7 +42431,7 @@
       <c r="G83" s="8"/>
       <c r="H83" s="8" cm="1">
         <f t="array" ref="H83">SUM(AA26:AE26*BR26:BV26-R26*BK26:BO26)</f>
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="I83" s="8" t="s">
         <v>25</v>
@@ -42085,7 +42443,7 @@
       <c r="L83" s="8"/>
       <c r="M83" s="8" cm="1">
         <f t="array" ref="M83">SUM(AA26:AE26*BR26:BV26-U26*BK26:BO26)</f>
-        <v>-15</v>
+        <v>-21</v>
       </c>
       <c r="N83" s="8" t="s">
         <v>21</v>
@@ -42414,7 +42772,7 @@
       <c r="G86" s="8"/>
       <c r="H86" s="8" cm="1">
         <f t="array" ref="H86">SUM(AA29:AE29*BR29:BV29-R29*BK29:BO29)</f>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="I86" s="8" t="s">
         <v>25</v>
@@ -42426,7 +42784,7 @@
       <c r="L86" s="8"/>
       <c r="M86" s="8" cm="1">
         <f t="array" ref="M86">SUM(AA29:AE29*BR29:BV29-U29*BK29:BO29)</f>
-        <v>-11</v>
+        <v>-6</v>
       </c>
       <c r="N86" s="8" t="s">
         <v>21</v>
@@ -42528,7 +42886,7 @@
       <c r="G87" s="8"/>
       <c r="H87" s="8" cm="1">
         <f t="array" ref="H87">SUM(AA30:AE30*BR30:BV30-R30*BK30:BO30)</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I87" s="8" t="s">
         <v>25</v>
@@ -42540,7 +42898,7 @@
       <c r="L87" s="8"/>
       <c r="M87" s="8" cm="1">
         <f t="array" ref="M87">SUM(AA30:AE30*BR30:BV30-U30*BK30:BO30)</f>
-        <v>-6</v>
+        <v>-8</v>
       </c>
       <c r="N87" s="8" t="s">
         <v>21</v>
@@ -42811,7 +43169,7 @@
       <c r="CL89" s="8"/>
       <c r="CM89" s="8"/>
     </row>
-    <row r="90" spans="1:91" ht="16.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:91" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A90" s="44"/>
       <c r="B90" s="25"/>
       <c r="C90" s="26"/>
@@ -44629,18 +44987,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -44776,6 +45134,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7F82F3A-971A-4E00-BEE7-5E3A8CB8E835}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E9105EF9-87DC-400D-AF3A-CEFE01235C70}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -44787,14 +45153,6 @@
     <ds:schemaRef ds:uri="b79073fe-1e48-4a97-9229-baaa8603d156"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7F82F3A-971A-4E00-BEE7-5E3A8CB8E835}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>